<commit_message>
Added the Vertex and Graph class.
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f472bcc8a8ceb2f6/Documents/Northeastern/Fall 2023/Algorithms/project/cs5800-project/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_360F29A56CC74F80DFBCDCCBEF94474CB64DABAD" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0A0AEC0-9626-4B68-8F43-75F29F1E2524}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
   <si>
     <t>Apres</t>
   </si>
@@ -63,19 +69,12 @@
   <si>
     <t>Stars &amp; Stripes</t>
   </si>
-  <si>
-    <t xml:space="preserve">Lone Pine </t>
-  </si>
-  <si>
-    <t>Stars and Stripes</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,6 +88,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -99,12 +104,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFd9ead3"/>
+        <fgColor rgb="FFD9EAD3"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFf4cccc"/>
+        <fgColor rgb="FFF4CCCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -125,16 +130,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </left>
       <right style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </right>
       <top style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -142,53 +147,51 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="12">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -199,10 +202,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
@@ -240,71 +243,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -332,7 +335,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -355,11 +358,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -368,13 +371,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -384,7 +387,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -393,7 +396,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -402,7 +405,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -410,10 +413,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -478,36 +481,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:Q75"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" style="10" width="14.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="11" width="5.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="11" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="11" width="11.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="11" width="9.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="11" width="14.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="11" width="7.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="11" width="12.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="11" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="11" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="11" width="10.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="11" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="11" width="6.433571428571429" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="11" width="9.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="11" width="11.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="11" width="7.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="12" width="13.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.54296875" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.54296875" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.81640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.81640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.1796875" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.7265625" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.1796875" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.81640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.453125" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.54296875" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.54296875" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.81640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.1796875" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -558,7 +563,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -611,7 +616,7 @@
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -664,7 +669,7 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -717,7 +722,7 @@
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -770,7 +775,7 @@
         <v>25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -823,7 +828,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -876,7 +881,7 @@
         <v>28</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -929,7 +934,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -982,9 +987,9 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row r="10" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B10" s="3">
         <v>4</v>
@@ -1035,7 +1040,7 @@
         <v>27</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row r="11" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1088,7 +1093,7 @@
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row r="12" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1141,7 +1146,7 @@
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row r="13" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1194,7 +1199,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row r="14" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1247,7 +1252,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row r="15" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>13</v>
       </c>
@@ -1300,7 +1305,7 @@
         <v>16</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row r="16" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1353,9 +1358,9 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row r="17" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" s="3">
         <v>23</v>
@@ -1406,8 +1411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="15.75">
-      <c r="A18" s="6"/>
+    <row r="18" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -1423,15 +1427,15 @@
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
       <c r="P18" s="3"/>
-      <c r="Q18" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="15.75">
-      <c r="A19" s="8"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
+      <c r="Q18" s="6"/>
+    </row>
+    <row r="19" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="7"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
@@ -1442,13 +1446,13 @@
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
       <c r="P19" s="3"/>
-      <c r="Q19" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="15.75">
+      <c r="Q19" s="6"/>
+    </row>
+    <row r="20" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="5"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -1461,10 +1465,9 @@
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
       <c r="P20" s="3"/>
-      <c r="Q20" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="15.75">
-      <c r="A21" s="6"/>
+      <c r="Q20" s="6"/>
+    </row>
+    <row r="21" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -1480,10 +1483,9 @@
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
       <c r="P21" s="3"/>
-      <c r="Q21" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="15.75">
-      <c r="A22" s="6"/>
+      <c r="Q21" s="6"/>
+    </row>
+    <row r="22" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -1499,10 +1501,9 @@
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
       <c r="P22" s="3"/>
-      <c r="Q22" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="15.75">
-      <c r="A23" s="6"/>
+      <c r="Q22" s="6"/>
+    </row>
+    <row r="23" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -1518,10 +1519,9 @@
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
-      <c r="Q23" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="15.75">
-      <c r="A24" s="6"/>
+      <c r="Q23" s="6"/>
+    </row>
+    <row r="24" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -1537,10 +1537,9 @@
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
       <c r="P24" s="3"/>
-      <c r="Q24" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="15.75">
-      <c r="A25" s="6"/>
+      <c r="Q24" s="6"/>
+    </row>
+    <row r="25" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -1556,10 +1555,9 @@
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
       <c r="P25" s="3"/>
-      <c r="Q25" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="15.75">
-      <c r="A26" s="6"/>
+      <c r="Q25" s="6"/>
+    </row>
+    <row r="26" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -1575,10 +1573,9 @@
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
-      <c r="Q26" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="15.75">
-      <c r="A27" s="6"/>
+      <c r="Q26" s="6"/>
+    </row>
+    <row r="27" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -1594,10 +1591,9 @@
       <c r="N27" s="3"/>
       <c r="O27" s="3"/>
       <c r="P27" s="3"/>
-      <c r="Q27" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="15.75">
-      <c r="A28" s="6"/>
+      <c r="Q27" s="6"/>
+    </row>
+    <row r="28" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -1613,10 +1609,9 @@
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
       <c r="P28" s="3"/>
-      <c r="Q28" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="15.75">
-      <c r="A29" s="6"/>
+      <c r="Q28" s="6"/>
+    </row>
+    <row r="29" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -1632,10 +1627,9 @@
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>
       <c r="P29" s="3"/>
-      <c r="Q29" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="15.75">
-      <c r="A30" s="6"/>
+      <c r="Q29" s="6"/>
+    </row>
+    <row r="30" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -1651,10 +1645,9 @@
       <c r="N30" s="3"/>
       <c r="O30" s="3"/>
       <c r="P30" s="3"/>
-      <c r="Q30" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="15.75">
-      <c r="A31" s="6"/>
+      <c r="Q30" s="6"/>
+    </row>
+    <row r="31" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -1670,10 +1663,9 @@
       <c r="N31" s="3"/>
       <c r="O31" s="3"/>
       <c r="P31" s="3"/>
-      <c r="Q31" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="15.75">
-      <c r="A32" s="6"/>
+      <c r="Q31" s="6"/>
+    </row>
+    <row r="32" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -1689,10 +1681,9 @@
       <c r="N32" s="3"/>
       <c r="O32" s="3"/>
       <c r="P32" s="3"/>
-      <c r="Q32" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="15.75">
-      <c r="A33" s="6"/>
+      <c r="Q32" s="6"/>
+    </row>
+    <row r="33" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
@@ -1708,10 +1699,9 @@
       <c r="N33" s="3"/>
       <c r="O33" s="3"/>
       <c r="P33" s="3"/>
-      <c r="Q33" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="15.75">
-      <c r="A34" s="6"/>
+      <c r="Q33" s="6"/>
+    </row>
+    <row r="34" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -1727,10 +1717,9 @@
       <c r="N34" s="3"/>
       <c r="O34" s="3"/>
       <c r="P34" s="3"/>
-      <c r="Q34" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="15.75">
-      <c r="A35" s="6"/>
+      <c r="Q34" s="6"/>
+    </row>
+    <row r="35" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
@@ -1746,10 +1735,9 @@
       <c r="N35" s="3"/>
       <c r="O35" s="3"/>
       <c r="P35" s="3"/>
-      <c r="Q35" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="15.75">
-      <c r="A36" s="6"/>
+      <c r="Q35" s="6"/>
+    </row>
+    <row r="36" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
@@ -1765,10 +1753,9 @@
       <c r="N36" s="3"/>
       <c r="O36" s="3"/>
       <c r="P36" s="3"/>
-      <c r="Q36" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="15.75">
-      <c r="A37" s="6"/>
+      <c r="Q36" s="6"/>
+    </row>
+    <row r="37" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -1784,10 +1771,9 @@
       <c r="N37" s="3"/>
       <c r="O37" s="3"/>
       <c r="P37" s="3"/>
-      <c r="Q37" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="15.75">
-      <c r="A38" s="6"/>
+      <c r="Q37" s="6"/>
+    </row>
+    <row r="38" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -1803,10 +1789,9 @@
       <c r="N38" s="3"/>
       <c r="O38" s="3"/>
       <c r="P38" s="3"/>
-      <c r="Q38" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="15.75">
-      <c r="A39" s="6"/>
+      <c r="Q38" s="6"/>
+    </row>
+    <row r="39" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -1822,10 +1807,9 @@
       <c r="N39" s="3"/>
       <c r="O39" s="3"/>
       <c r="P39" s="3"/>
-      <c r="Q39" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="15.75">
-      <c r="A40" s="6"/>
+      <c r="Q39" s="6"/>
+    </row>
+    <row r="40" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
@@ -1841,10 +1825,9 @@
       <c r="N40" s="3"/>
       <c r="O40" s="3"/>
       <c r="P40" s="3"/>
-      <c r="Q40" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="15.75">
-      <c r="A41" s="6"/>
+      <c r="Q40" s="6"/>
+    </row>
+    <row r="41" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
@@ -1860,10 +1843,9 @@
       <c r="N41" s="3"/>
       <c r="O41" s="3"/>
       <c r="P41" s="3"/>
-      <c r="Q41" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
-      <c r="A42" s="6"/>
+      <c r="Q41" s="6"/>
+    </row>
+    <row r="42" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
@@ -1879,10 +1861,9 @@
       <c r="N42" s="3"/>
       <c r="O42" s="3"/>
       <c r="P42" s="3"/>
-      <c r="Q42" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
-      <c r="A43" s="6"/>
+      <c r="Q42" s="6"/>
+    </row>
+    <row r="43" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
@@ -1898,10 +1879,9 @@
       <c r="N43" s="3"/>
       <c r="O43" s="3"/>
       <c r="P43" s="3"/>
-      <c r="Q43" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
-      <c r="A44" s="6"/>
+      <c r="Q43" s="6"/>
+    </row>
+    <row r="44" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
@@ -1917,10 +1897,9 @@
       <c r="N44" s="3"/>
       <c r="O44" s="3"/>
       <c r="P44" s="3"/>
-      <c r="Q44" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
-      <c r="A45" s="6"/>
+      <c r="Q44" s="6"/>
+    </row>
+    <row r="45" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
@@ -1936,10 +1915,9 @@
       <c r="N45" s="3"/>
       <c r="O45" s="3"/>
       <c r="P45" s="3"/>
-      <c r="Q45" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
-      <c r="A46" s="6"/>
+      <c r="Q45" s="6"/>
+    </row>
+    <row r="46" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
@@ -1955,10 +1933,9 @@
       <c r="N46" s="3"/>
       <c r="O46" s="3"/>
       <c r="P46" s="3"/>
-      <c r="Q46" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
-      <c r="A47" s="6"/>
+      <c r="Q46" s="6"/>
+    </row>
+    <row r="47" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
@@ -1974,10 +1951,9 @@
       <c r="N47" s="3"/>
       <c r="O47" s="3"/>
       <c r="P47" s="3"/>
-      <c r="Q47" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
-      <c r="A48" s="6"/>
+      <c r="Q47" s="6"/>
+    </row>
+    <row r="48" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
@@ -1993,10 +1969,9 @@
       <c r="N48" s="3"/>
       <c r="O48" s="3"/>
       <c r="P48" s="3"/>
-      <c r="Q48" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
-      <c r="A49" s="6"/>
+      <c r="Q48" s="6"/>
+    </row>
+    <row r="49" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
@@ -2012,10 +1987,9 @@
       <c r="N49" s="3"/>
       <c r="O49" s="3"/>
       <c r="P49" s="3"/>
-      <c r="Q49" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
-      <c r="A50" s="6"/>
+      <c r="Q49" s="6"/>
+    </row>
+    <row r="50" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
@@ -2031,10 +2005,9 @@
       <c r="N50" s="3"/>
       <c r="O50" s="3"/>
       <c r="P50" s="3"/>
-      <c r="Q50" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
-      <c r="A51" s="6"/>
+      <c r="Q50" s="6"/>
+    </row>
+    <row r="51" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
@@ -2050,10 +2023,9 @@
       <c r="N51" s="3"/>
       <c r="O51" s="3"/>
       <c r="P51" s="3"/>
-      <c r="Q51" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
-      <c r="A52" s="6"/>
+      <c r="Q51" s="6"/>
+    </row>
+    <row r="52" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
@@ -2069,10 +2041,9 @@
       <c r="N52" s="3"/>
       <c r="O52" s="3"/>
       <c r="P52" s="3"/>
-      <c r="Q52" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
-      <c r="A53" s="6"/>
+      <c r="Q52" s="6"/>
+    </row>
+    <row r="53" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
@@ -2088,10 +2059,9 @@
       <c r="N53" s="3"/>
       <c r="O53" s="3"/>
       <c r="P53" s="3"/>
-      <c r="Q53" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
-      <c r="A54" s="6"/>
+      <c r="Q53" s="6"/>
+    </row>
+    <row r="54" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
@@ -2107,10 +2077,9 @@
       <c r="N54" s="3"/>
       <c r="O54" s="3"/>
       <c r="P54" s="3"/>
-      <c r="Q54" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
-      <c r="A55" s="6"/>
+      <c r="Q54" s="6"/>
+    </row>
+    <row r="55" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
@@ -2126,10 +2095,9 @@
       <c r="N55" s="3"/>
       <c r="O55" s="3"/>
       <c r="P55" s="3"/>
-      <c r="Q55" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
-      <c r="A56" s="6"/>
+      <c r="Q55" s="6"/>
+    </row>
+    <row r="56" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
@@ -2145,10 +2113,9 @@
       <c r="N56" s="3"/>
       <c r="O56" s="3"/>
       <c r="P56" s="3"/>
-      <c r="Q56" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
-      <c r="A57" s="6"/>
+      <c r="Q56" s="6"/>
+    </row>
+    <row r="57" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
@@ -2164,10 +2131,9 @@
       <c r="N57" s="3"/>
       <c r="O57" s="3"/>
       <c r="P57" s="3"/>
-      <c r="Q57" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
-      <c r="A58" s="6"/>
+      <c r="Q57" s="6"/>
+    </row>
+    <row r="58" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
@@ -2183,10 +2149,9 @@
       <c r="N58" s="3"/>
       <c r="O58" s="3"/>
       <c r="P58" s="3"/>
-      <c r="Q58" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
-      <c r="A59" s="6"/>
+      <c r="Q58" s="6"/>
+    </row>
+    <row r="59" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
@@ -2202,10 +2167,9 @@
       <c r="N59" s="3"/>
       <c r="O59" s="3"/>
       <c r="P59" s="3"/>
-      <c r="Q59" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
-      <c r="A60" s="6"/>
+      <c r="Q59" s="6"/>
+    </row>
+    <row r="60" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
@@ -2221,10 +2185,9 @@
       <c r="N60" s="3"/>
       <c r="O60" s="3"/>
       <c r="P60" s="3"/>
-      <c r="Q60" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
-      <c r="A61" s="6"/>
+      <c r="Q60" s="6"/>
+    </row>
+    <row r="61" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
@@ -2240,10 +2203,9 @@
       <c r="N61" s="3"/>
       <c r="O61" s="3"/>
       <c r="P61" s="3"/>
-      <c r="Q61" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
-      <c r="A62" s="6"/>
+      <c r="Q61" s="6"/>
+    </row>
+    <row r="62" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
@@ -2259,10 +2221,9 @@
       <c r="N62" s="3"/>
       <c r="O62" s="3"/>
       <c r="P62" s="3"/>
-      <c r="Q62" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
-      <c r="A63" s="6"/>
+      <c r="Q62" s="6"/>
+    </row>
+    <row r="63" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
@@ -2278,10 +2239,9 @@
       <c r="N63" s="3"/>
       <c r="O63" s="3"/>
       <c r="P63" s="3"/>
-      <c r="Q63" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
-      <c r="A64" s="6"/>
+      <c r="Q63" s="6"/>
+    </row>
+    <row r="64" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
@@ -2297,10 +2257,9 @@
       <c r="N64" s="3"/>
       <c r="O64" s="3"/>
       <c r="P64" s="3"/>
-      <c r="Q64" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
-      <c r="A65" s="6"/>
+      <c r="Q64" s="6"/>
+    </row>
+    <row r="65" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
@@ -2316,10 +2275,9 @@
       <c r="N65" s="3"/>
       <c r="O65" s="3"/>
       <c r="P65" s="3"/>
-      <c r="Q65" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
-      <c r="A66" s="6"/>
+      <c r="Q65" s="6"/>
+    </row>
+    <row r="66" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
@@ -2335,10 +2293,9 @@
       <c r="N66" s="3"/>
       <c r="O66" s="3"/>
       <c r="P66" s="3"/>
-      <c r="Q66" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
-      <c r="A67" s="6"/>
+      <c r="Q66" s="6"/>
+    </row>
+    <row r="67" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
@@ -2354,10 +2311,9 @@
       <c r="N67" s="3"/>
       <c r="O67" s="3"/>
       <c r="P67" s="3"/>
-      <c r="Q67" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
-      <c r="A68" s="6"/>
+      <c r="Q67" s="6"/>
+    </row>
+    <row r="68" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
@@ -2373,10 +2329,9 @@
       <c r="N68" s="3"/>
       <c r="O68" s="3"/>
       <c r="P68" s="3"/>
-      <c r="Q68" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
-      <c r="A69" s="6"/>
+      <c r="Q68" s="6"/>
+    </row>
+    <row r="69" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
@@ -2392,10 +2347,9 @@
       <c r="N69" s="3"/>
       <c r="O69" s="3"/>
       <c r="P69" s="3"/>
-      <c r="Q69" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
-      <c r="A70" s="6"/>
+      <c r="Q69" s="6"/>
+    </row>
+    <row r="70" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
@@ -2411,10 +2365,9 @@
       <c r="N70" s="3"/>
       <c r="O70" s="3"/>
       <c r="P70" s="3"/>
-      <c r="Q70" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
-      <c r="A71" s="6"/>
+      <c r="Q70" s="6"/>
+    </row>
+    <row r="71" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
       <c r="D71" s="3"/>
@@ -2430,10 +2383,9 @@
       <c r="N71" s="3"/>
       <c r="O71" s="3"/>
       <c r="P71" s="3"/>
-      <c r="Q71" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
-      <c r="A72" s="6"/>
+      <c r="Q71" s="6"/>
+    </row>
+    <row r="72" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
       <c r="D72" s="3"/>
@@ -2449,10 +2401,9 @@
       <c r="N72" s="3"/>
       <c r="O72" s="3"/>
       <c r="P72" s="3"/>
-      <c r="Q72" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
-      <c r="A73" s="6"/>
+      <c r="Q72" s="6"/>
+    </row>
+    <row r="73" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
@@ -2468,10 +2419,9 @@
       <c r="N73" s="3"/>
       <c r="O73" s="3"/>
       <c r="P73" s="3"/>
-      <c r="Q73" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
-      <c r="A74" s="6"/>
+      <c r="Q73" s="6"/>
+    </row>
+    <row r="74" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
       <c r="D74" s="3"/>
@@ -2487,10 +2437,9 @@
       <c r="N74" s="3"/>
       <c r="O74" s="3"/>
       <c r="P74" s="3"/>
-      <c r="Q74" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75">
-      <c r="A75" s="6"/>
+      <c r="Q74" s="6"/>
+    </row>
+    <row r="75" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
       <c r="D75" s="3"/>
@@ -2506,7 +2455,7 @@
       <c r="N75" s="3"/>
       <c r="O75" s="3"/>
       <c r="P75" s="3"/>
-      <c r="Q75" s="7"/>
+      <c r="Q75" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Adapting nearest neighbor with some constraints.
- Put Graph and Vertices classes in their own separate files.
- Adapted Dan's implementation of the nearest neighbor and Dijskstra algorithm into the crawl function
- implemented some basic constraints that allows for some more control over the graph traversal. Like max number of breweries to visit, max walking time, and overall time limits.
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f472bcc8a8ceb2f6/Documents/Northeastern/Fall 2023/Algorithms/project/cs5800-project/data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_360F29A56CC74F80DFBCDCCBEF94474CB64DABAD" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0A0AEC0-9626-4B68-8F43-75F29F1E2524}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -73,7 +67,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -90,7 +85,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -104,12 +99,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD9EAD3"/>
+        <fgColor rgb="FFd9ead3"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF4CCCC"/>
+        <fgColor rgb="FFf4cccc"/>
       </patternFill>
     </fill>
   </fills>
@@ -130,16 +125,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </left>
       <right style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </right>
       <top style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -147,51 +142,53 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="13">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -202,10 +199,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
@@ -243,71 +240,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -335,7 +332,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -358,11 +355,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -371,13 +368,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -387,7 +384,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -396,7 +393,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -405,7 +402,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -413,10 +410,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -481,38 +478,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:Q75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.54296875" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1796875" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.54296875" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.26953125" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.81640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.81640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.1796875" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.7265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.1796875" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.81640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.453125" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.54296875" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.54296875" style="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.81640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.1796875" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="10" width="14.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="11" width="5.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="11" width="11.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="11" width="11.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="11" width="9.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="11" width="14.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="11" width="7.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="11" width="12.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="11" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="11" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="11" width="10.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="11" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="11" width="6.433571428571429" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="11" width="9.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="11" width="11.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="11" width="7.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="12" width="13.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -563,7 +558,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -606,9 +601,7 @@
       <c r="N2" s="3">
         <v>4</v>
       </c>
-      <c r="O2" s="3">
-        <v>18</v>
-      </c>
+      <c r="O2" s="3"/>
       <c r="P2" s="3">
         <v>16</v>
       </c>
@@ -616,7 +609,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -659,9 +652,7 @@
       <c r="N3" s="3">
         <v>1</v>
       </c>
-      <c r="O3" s="3">
-        <v>18</v>
-      </c>
+      <c r="O3" s="3"/>
       <c r="P3" s="3">
         <v>15</v>
       </c>
@@ -669,7 +660,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -712,9 +703,7 @@
       <c r="N4" s="3">
         <v>13</v>
       </c>
-      <c r="O4" s="3">
-        <v>27</v>
-      </c>
+      <c r="O4" s="3"/>
       <c r="P4" s="3">
         <v>24</v>
       </c>
@@ -722,7 +711,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -765,9 +754,7 @@
       <c r="N5" s="3">
         <v>6</v>
       </c>
-      <c r="O5" s="3">
-        <v>20</v>
-      </c>
+      <c r="O5" s="3"/>
       <c r="P5" s="3">
         <v>18</v>
       </c>
@@ -775,7 +762,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -818,9 +805,7 @@
       <c r="N6" s="3">
         <v>16</v>
       </c>
-      <c r="O6" s="3">
-        <v>6</v>
-      </c>
+      <c r="O6" s="3"/>
       <c r="P6" s="3">
         <v>6</v>
       </c>
@@ -828,7 +813,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -871,9 +856,7 @@
       <c r="N7" s="3">
         <v>8</v>
       </c>
-      <c r="O7" s="3">
-        <v>22</v>
-      </c>
+      <c r="O7" s="3"/>
       <c r="P7" s="3">
         <v>21</v>
       </c>
@@ -881,7 +864,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -924,9 +907,7 @@
       <c r="N8" s="3">
         <v>20</v>
       </c>
-      <c r="O8" s="3">
-        <v>12</v>
-      </c>
+      <c r="O8" s="3"/>
       <c r="P8" s="3">
         <v>12</v>
       </c>
@@ -934,7 +915,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -977,9 +958,7 @@
       <c r="N9" s="3">
         <v>23</v>
       </c>
-      <c r="O9" s="3">
-        <v>15</v>
-      </c>
+      <c r="O9" s="3"/>
       <c r="P9" s="3">
         <v>15</v>
       </c>
@@ -987,7 +966,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1030,9 +1009,7 @@
       <c r="N10" s="3">
         <v>8</v>
       </c>
-      <c r="O10" s="3">
-        <v>21</v>
-      </c>
+      <c r="O10" s="3"/>
       <c r="P10" s="3">
         <v>20</v>
       </c>
@@ -1040,7 +1017,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1083,9 +1060,7 @@
       <c r="N11" s="3">
         <v>7</v>
       </c>
-      <c r="O11" s="3">
-        <v>16</v>
-      </c>
+      <c r="O11" s="3"/>
       <c r="P11" s="3">
         <v>15</v>
       </c>
@@ -1093,7 +1068,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1136,9 +1111,7 @@
       <c r="N12" s="3">
         <v>3</v>
       </c>
-      <c r="O12" s="3">
-        <v>18</v>
-      </c>
+      <c r="O12" s="3"/>
       <c r="P12" s="3">
         <v>16</v>
       </c>
@@ -1146,7 +1119,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1189,9 +1162,7 @@
       <c r="N13" s="3">
         <v>8</v>
       </c>
-      <c r="O13" s="3">
-        <v>10</v>
-      </c>
+      <c r="O13" s="3"/>
       <c r="P13" s="3">
         <v>9</v>
       </c>
@@ -1199,7 +1170,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1242,9 +1213,7 @@
       <c r="N14" s="3">
         <v>0</v>
       </c>
-      <c r="O14" s="3">
-        <v>18</v>
-      </c>
+      <c r="O14" s="3"/>
       <c r="P14" s="3">
         <v>15</v>
       </c>
@@ -1252,7 +1221,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="5" t="s">
         <v>13</v>
       </c>
@@ -1295,9 +1264,7 @@
       <c r="N15" s="3">
         <v>18</v>
       </c>
-      <c r="O15" s="3">
-        <v>0</v>
-      </c>
+      <c r="O15" s="3"/>
       <c r="P15" s="3">
         <v>4</v>
       </c>
@@ -1305,7 +1272,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1348,9 +1315,7 @@
       <c r="N16" s="3">
         <v>15</v>
       </c>
-      <c r="O16" s="3">
-        <v>4</v>
-      </c>
+      <c r="O16" s="3"/>
       <c r="P16" s="3">
         <v>0</v>
       </c>
@@ -1358,7 +1323,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -1401,9 +1366,7 @@
       <c r="N17" s="3">
         <v>20</v>
       </c>
-      <c r="O17" s="3">
-        <v>16</v>
-      </c>
+      <c r="O17" s="3"/>
       <c r="P17" s="3">
         <v>13</v>
       </c>
@@ -1411,7 +1374,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+      <c r="A18" s="6"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -1427,15 +1391,15 @@
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
       <c r="P18" s="3"/>
-      <c r="Q18" s="6"/>
-    </row>
-    <row r="19" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="7"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
+      <c r="Q18" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+      <c r="A19" s="8"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
@@ -1446,13 +1410,13 @@
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
       <c r="P19" s="3"/>
-      <c r="Q19" s="6"/>
-    </row>
-    <row r="20" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q19" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="5"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -1465,9 +1429,10 @@
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
       <c r="P20" s="3"/>
-      <c r="Q20" s="6"/>
-    </row>
-    <row r="21" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q20" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
+      <c r="A21" s="6"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -1483,9 +1448,10 @@
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
       <c r="P21" s="3"/>
-      <c r="Q21" s="6"/>
-    </row>
-    <row r="22" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q21" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
+      <c r="A22" s="6"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -1501,9 +1467,10 @@
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
       <c r="P22" s="3"/>
-      <c r="Q22" s="6"/>
-    </row>
-    <row r="23" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q22" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
+      <c r="A23" s="6"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -1519,9 +1486,10 @@
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
-      <c r="Q23" s="6"/>
-    </row>
-    <row r="24" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q23" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
+      <c r="A24" s="6"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -1537,9 +1505,10 @@
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
       <c r="P24" s="3"/>
-      <c r="Q24" s="6"/>
-    </row>
-    <row r="25" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q24" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
+      <c r="A25" s="6"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -1555,9 +1524,10 @@
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
       <c r="P25" s="3"/>
-      <c r="Q25" s="6"/>
-    </row>
-    <row r="26" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q25" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
+      <c r="A26" s="6"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -1573,9 +1543,10 @@
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
-      <c r="Q26" s="6"/>
-    </row>
-    <row r="27" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q26" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
+      <c r="A27" s="6"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -1591,9 +1562,10 @@
       <c r="N27" s="3"/>
       <c r="O27" s="3"/>
       <c r="P27" s="3"/>
-      <c r="Q27" s="6"/>
-    </row>
-    <row r="28" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q27" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
+      <c r="A28" s="6"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -1609,9 +1581,10 @@
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
       <c r="P28" s="3"/>
-      <c r="Q28" s="6"/>
-    </row>
-    <row r="29" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q28" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
+      <c r="A29" s="6"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -1627,9 +1600,10 @@
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>
       <c r="P29" s="3"/>
-      <c r="Q29" s="6"/>
-    </row>
-    <row r="30" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q29" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
+      <c r="A30" s="6"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -1645,9 +1619,10 @@
       <c r="N30" s="3"/>
       <c r="O30" s="3"/>
       <c r="P30" s="3"/>
-      <c r="Q30" s="6"/>
-    </row>
-    <row r="31" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q30" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
+      <c r="A31" s="6"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -1663,9 +1638,10 @@
       <c r="N31" s="3"/>
       <c r="O31" s="3"/>
       <c r="P31" s="3"/>
-      <c r="Q31" s="6"/>
-    </row>
-    <row r="32" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q31" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
+      <c r="A32" s="6"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -1681,9 +1657,10 @@
       <c r="N32" s="3"/>
       <c r="O32" s="3"/>
       <c r="P32" s="3"/>
-      <c r="Q32" s="6"/>
-    </row>
-    <row r="33" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q32" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
+      <c r="A33" s="6"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
@@ -1699,9 +1676,10 @@
       <c r="N33" s="3"/>
       <c r="O33" s="3"/>
       <c r="P33" s="3"/>
-      <c r="Q33" s="6"/>
-    </row>
-    <row r="34" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q33" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="15.75">
+      <c r="A34" s="6"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -1717,9 +1695,10 @@
       <c r="N34" s="3"/>
       <c r="O34" s="3"/>
       <c r="P34" s="3"/>
-      <c r="Q34" s="6"/>
-    </row>
-    <row r="35" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q34" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="15.75">
+      <c r="A35" s="6"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
@@ -1735,9 +1714,10 @@
       <c r="N35" s="3"/>
       <c r="O35" s="3"/>
       <c r="P35" s="3"/>
-      <c r="Q35" s="6"/>
-    </row>
-    <row r="36" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q35" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="15.75">
+      <c r="A36" s="6"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
@@ -1753,9 +1733,10 @@
       <c r="N36" s="3"/>
       <c r="O36" s="3"/>
       <c r="P36" s="3"/>
-      <c r="Q36" s="6"/>
-    </row>
-    <row r="37" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q36" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="15.75">
+      <c r="A37" s="6"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -1771,9 +1752,10 @@
       <c r="N37" s="3"/>
       <c r="O37" s="3"/>
       <c r="P37" s="3"/>
-      <c r="Q37" s="6"/>
-    </row>
-    <row r="38" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q37" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="15.75">
+      <c r="A38" s="6"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -1789,9 +1771,10 @@
       <c r="N38" s="3"/>
       <c r="O38" s="3"/>
       <c r="P38" s="3"/>
-      <c r="Q38" s="6"/>
-    </row>
-    <row r="39" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q38" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="15.75">
+      <c r="A39" s="6"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -1807,9 +1790,10 @@
       <c r="N39" s="3"/>
       <c r="O39" s="3"/>
       <c r="P39" s="3"/>
-      <c r="Q39" s="6"/>
-    </row>
-    <row r="40" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q39" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="15.75">
+      <c r="A40" s="6"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
@@ -1825,9 +1809,10 @@
       <c r="N40" s="3"/>
       <c r="O40" s="3"/>
       <c r="P40" s="3"/>
-      <c r="Q40" s="6"/>
-    </row>
-    <row r="41" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q40" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="15.75">
+      <c r="A41" s="6"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
@@ -1843,9 +1828,10 @@
       <c r="N41" s="3"/>
       <c r="O41" s="3"/>
       <c r="P41" s="3"/>
-      <c r="Q41" s="6"/>
-    </row>
-    <row r="42" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q41" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
+      <c r="A42" s="6"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
@@ -1861,9 +1847,10 @@
       <c r="N42" s="3"/>
       <c r="O42" s="3"/>
       <c r="P42" s="3"/>
-      <c r="Q42" s="6"/>
-    </row>
-    <row r="43" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q42" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
+      <c r="A43" s="6"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
@@ -1879,9 +1866,10 @@
       <c r="N43" s="3"/>
       <c r="O43" s="3"/>
       <c r="P43" s="3"/>
-      <c r="Q43" s="6"/>
-    </row>
-    <row r="44" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q43" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
+      <c r="A44" s="6"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
@@ -1897,9 +1885,10 @@
       <c r="N44" s="3"/>
       <c r="O44" s="3"/>
       <c r="P44" s="3"/>
-      <c r="Q44" s="6"/>
-    </row>
-    <row r="45" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q44" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
+      <c r="A45" s="6"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
@@ -1915,9 +1904,10 @@
       <c r="N45" s="3"/>
       <c r="O45" s="3"/>
       <c r="P45" s="3"/>
-      <c r="Q45" s="6"/>
-    </row>
-    <row r="46" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q45" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
+      <c r="A46" s="6"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
@@ -1933,9 +1923,10 @@
       <c r="N46" s="3"/>
       <c r="O46" s="3"/>
       <c r="P46" s="3"/>
-      <c r="Q46" s="6"/>
-    </row>
-    <row r="47" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q46" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
+      <c r="A47" s="6"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
@@ -1951,9 +1942,10 @@
       <c r="N47" s="3"/>
       <c r="O47" s="3"/>
       <c r="P47" s="3"/>
-      <c r="Q47" s="6"/>
-    </row>
-    <row r="48" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q47" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
+      <c r="A48" s="6"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
@@ -1969,9 +1961,10 @@
       <c r="N48" s="3"/>
       <c r="O48" s="3"/>
       <c r="P48" s="3"/>
-      <c r="Q48" s="6"/>
-    </row>
-    <row r="49" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q48" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
+      <c r="A49" s="6"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
@@ -1987,9 +1980,10 @@
       <c r="N49" s="3"/>
       <c r="O49" s="3"/>
       <c r="P49" s="3"/>
-      <c r="Q49" s="6"/>
-    </row>
-    <row r="50" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q49" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
+      <c r="A50" s="6"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
@@ -2005,9 +1999,10 @@
       <c r="N50" s="3"/>
       <c r="O50" s="3"/>
       <c r="P50" s="3"/>
-      <c r="Q50" s="6"/>
-    </row>
-    <row r="51" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q50" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
+      <c r="A51" s="6"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
@@ -2023,9 +2018,10 @@
       <c r="N51" s="3"/>
       <c r="O51" s="3"/>
       <c r="P51" s="3"/>
-      <c r="Q51" s="6"/>
-    </row>
-    <row r="52" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q51" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
+      <c r="A52" s="6"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
@@ -2041,9 +2037,10 @@
       <c r="N52" s="3"/>
       <c r="O52" s="3"/>
       <c r="P52" s="3"/>
-      <c r="Q52" s="6"/>
-    </row>
-    <row r="53" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q52" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
+      <c r="A53" s="6"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
@@ -2059,9 +2056,10 @@
       <c r="N53" s="3"/>
       <c r="O53" s="3"/>
       <c r="P53" s="3"/>
-      <c r="Q53" s="6"/>
-    </row>
-    <row r="54" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q53" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
+      <c r="A54" s="6"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
@@ -2077,9 +2075,10 @@
       <c r="N54" s="3"/>
       <c r="O54" s="3"/>
       <c r="P54" s="3"/>
-      <c r="Q54" s="6"/>
-    </row>
-    <row r="55" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q54" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
+      <c r="A55" s="6"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
@@ -2095,9 +2094,10 @@
       <c r="N55" s="3"/>
       <c r="O55" s="3"/>
       <c r="P55" s="3"/>
-      <c r="Q55" s="6"/>
-    </row>
-    <row r="56" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q55" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
+      <c r="A56" s="6"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
@@ -2113,9 +2113,10 @@
       <c r="N56" s="3"/>
       <c r="O56" s="3"/>
       <c r="P56" s="3"/>
-      <c r="Q56" s="6"/>
-    </row>
-    <row r="57" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q56" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
+      <c r="A57" s="6"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
@@ -2131,9 +2132,10 @@
       <c r="N57" s="3"/>
       <c r="O57" s="3"/>
       <c r="P57" s="3"/>
-      <c r="Q57" s="6"/>
-    </row>
-    <row r="58" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q57" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
+      <c r="A58" s="6"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
@@ -2149,9 +2151,10 @@
       <c r="N58" s="3"/>
       <c r="O58" s="3"/>
       <c r="P58" s="3"/>
-      <c r="Q58" s="6"/>
-    </row>
-    <row r="59" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q58" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
+      <c r="A59" s="6"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
@@ -2167,9 +2170,10 @@
       <c r="N59" s="3"/>
       <c r="O59" s="3"/>
       <c r="P59" s="3"/>
-      <c r="Q59" s="6"/>
-    </row>
-    <row r="60" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q59" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
+      <c r="A60" s="6"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
@@ -2185,9 +2189,10 @@
       <c r="N60" s="3"/>
       <c r="O60" s="3"/>
       <c r="P60" s="3"/>
-      <c r="Q60" s="6"/>
-    </row>
-    <row r="61" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q60" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
+      <c r="A61" s="6"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
@@ -2203,9 +2208,10 @@
       <c r="N61" s="3"/>
       <c r="O61" s="3"/>
       <c r="P61" s="3"/>
-      <c r="Q61" s="6"/>
-    </row>
-    <row r="62" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q61" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
+      <c r="A62" s="6"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
@@ -2221,9 +2227,10 @@
       <c r="N62" s="3"/>
       <c r="O62" s="3"/>
       <c r="P62" s="3"/>
-      <c r="Q62" s="6"/>
-    </row>
-    <row r="63" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q62" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
+      <c r="A63" s="6"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
@@ -2239,9 +2246,10 @@
       <c r="N63" s="3"/>
       <c r="O63" s="3"/>
       <c r="P63" s="3"/>
-      <c r="Q63" s="6"/>
-    </row>
-    <row r="64" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q63" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
+      <c r="A64" s="6"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
@@ -2257,9 +2265,10 @@
       <c r="N64" s="3"/>
       <c r="O64" s="3"/>
       <c r="P64" s="3"/>
-      <c r="Q64" s="6"/>
-    </row>
-    <row r="65" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q64" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
+      <c r="A65" s="6"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
@@ -2275,9 +2284,10 @@
       <c r="N65" s="3"/>
       <c r="O65" s="3"/>
       <c r="P65" s="3"/>
-      <c r="Q65" s="6"/>
-    </row>
-    <row r="66" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q65" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
+      <c r="A66" s="6"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
@@ -2293,9 +2303,10 @@
       <c r="N66" s="3"/>
       <c r="O66" s="3"/>
       <c r="P66" s="3"/>
-      <c r="Q66" s="6"/>
-    </row>
-    <row r="67" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q66" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
+      <c r="A67" s="6"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
@@ -2311,9 +2322,10 @@
       <c r="N67" s="3"/>
       <c r="O67" s="3"/>
       <c r="P67" s="3"/>
-      <c r="Q67" s="6"/>
-    </row>
-    <row r="68" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q67" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
+      <c r="A68" s="6"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
@@ -2329,9 +2341,10 @@
       <c r="N68" s="3"/>
       <c r="O68" s="3"/>
       <c r="P68" s="3"/>
-      <c r="Q68" s="6"/>
-    </row>
-    <row r="69" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q68" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
+      <c r="A69" s="6"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
@@ -2347,9 +2360,10 @@
       <c r="N69" s="3"/>
       <c r="O69" s="3"/>
       <c r="P69" s="3"/>
-      <c r="Q69" s="6"/>
-    </row>
-    <row r="70" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q69" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
+      <c r="A70" s="6"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
@@ -2365,9 +2379,10 @@
       <c r="N70" s="3"/>
       <c r="O70" s="3"/>
       <c r="P70" s="3"/>
-      <c r="Q70" s="6"/>
-    </row>
-    <row r="71" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q70" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
+      <c r="A71" s="6"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
       <c r="D71" s="3"/>
@@ -2383,9 +2398,10 @@
       <c r="N71" s="3"/>
       <c r="O71" s="3"/>
       <c r="P71" s="3"/>
-      <c r="Q71" s="6"/>
-    </row>
-    <row r="72" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q71" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
+      <c r="A72" s="6"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
       <c r="D72" s="3"/>
@@ -2401,9 +2417,10 @@
       <c r="N72" s="3"/>
       <c r="O72" s="3"/>
       <c r="P72" s="3"/>
-      <c r="Q72" s="6"/>
-    </row>
-    <row r="73" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q72" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
+      <c r="A73" s="6"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
@@ -2419,9 +2436,10 @@
       <c r="N73" s="3"/>
       <c r="O73" s="3"/>
       <c r="P73" s="3"/>
-      <c r="Q73" s="6"/>
-    </row>
-    <row r="74" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q73" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
+      <c r="A74" s="6"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
       <c r="D74" s="3"/>
@@ -2437,9 +2455,10 @@
       <c r="N74" s="3"/>
       <c r="O74" s="3"/>
       <c r="P74" s="3"/>
-      <c r="Q74" s="6"/>
-    </row>
-    <row r="75" spans="2:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q74" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75">
+      <c r="A75" s="6"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
       <c r="D75" s="3"/>
@@ -2455,7 +2474,7 @@
       <c r="N75" s="3"/>
       <c r="O75" s="3"/>
       <c r="P75" s="3"/>
-      <c r="Q75" s="6"/>
+      <c r="Q75" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>